<commit_message>
Added a --url param so you can specify a distribution. Only working for the spreadsheet mode at the moment
</commit_message>
<xml_diff>
--- a/test_data/Glop_Pot/CATALOG_glop_pot.xlsx
+++ b/test_data/Glop_Pot/CATALOG_glop_pot.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/124411/Dropbox/calcyte.js/test_data/Glop_Pot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{2EA5F41F-45D0-1543-8FF1-5A7CADBBC1DA}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{FB16824F-EDB7-E04C-8751-346D484730DD}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Collection" sheetId="1" r:id="rId1"/>
@@ -615,8 +615,8 @@
   <sheetPr codeName="Collection"/>
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -902,7 +902,9 @@
   <sheetPr codeName="Places"/>
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -1046,7 +1048,7 @@
   <sheetPr codeName="Organizations"/>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Now passing all but 2 of tests
</commit_message>
<xml_diff>
--- a/test_data/Glop_Pot/CATALOG_glop_pot.xlsx
+++ b/test_data/Glop_Pot/CATALOG_glop_pot.xlsx
@@ -486,7 +486,7 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Files"/>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -504,6 +504,9 @@
       <c r="D1" t="str">
         <v>RELATION:License</v>
       </c>
+      <c r="E1" t="str">
+        <v>*MISSING-FILE*</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
@@ -531,6 +534,30 @@
       </c>
       <c r="D3" t="str">
         <v>CC-BY</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>sftest.json</v>
+      </c>
+      <c r="E4" t="str">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>test.sf.json</v>
+      </c>
+      <c r="E5" t="str">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>test.sf.pp.json</v>
+      </c>
+      <c r="E6" t="str">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>